<commit_message>
update planilha UAT | incompleta
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de Testes (UAT).xlsx
+++ b/Documentação/Planilha de Testes (UAT).xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghgoncalves\Desktop\project-hunter\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5167849D-1CA6-44DC-A049-1CEB382A046A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96884328-CD11-4780-AF59-3F536C1507E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{CCEB0146-9C4B-423C-9F76-223A38A39EE4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{CCEB0146-9C4B-423C-9F76-223A38A39EE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="3" r:id="rId1"/>
-    <sheet name="Recuperação de Senha" sheetId="2" r:id="rId2"/>
-    <sheet name="Cadastro" sheetId="11" r:id="rId3"/>
-    <sheet name="Continuação do Cadastro" sheetId="8" r:id="rId4"/>
-    <sheet name="Home" sheetId="4" r:id="rId5"/>
-    <sheet name="Configurações" sheetId="5" r:id="rId6"/>
-    <sheet name="Perfil do Jogador" sheetId="6" r:id="rId7"/>
-    <sheet name="Perfil da Equipe" sheetId="7" r:id="rId8"/>
-    <sheet name="Buscar" sheetId="9" r:id="rId9"/>
-    <sheet name="Agendamento de Partida" sheetId="10" r:id="rId10"/>
+    <sheet name="Login (Erro)" sheetId="12" r:id="rId2"/>
+    <sheet name="Recuperação de Senha" sheetId="2" r:id="rId3"/>
+    <sheet name="Cadastro" sheetId="11" r:id="rId4"/>
+    <sheet name="Cadastro (Erro)" sheetId="13" r:id="rId5"/>
+    <sheet name="Continuação do Cadastro" sheetId="8" r:id="rId6"/>
+    <sheet name="Home" sheetId="4" r:id="rId7"/>
+    <sheet name="Configurações" sheetId="5" r:id="rId8"/>
+    <sheet name="Perfil do Jogador" sheetId="6" r:id="rId9"/>
+    <sheet name="Perfil da Equipe" sheetId="7" r:id="rId10"/>
+    <sheet name="Buscar" sheetId="9" r:id="rId11"/>
+    <sheet name="Agendamento de Partida" sheetId="10" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,9 +34,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="62">
   <si>
     <t>UAT_A_001</t>
   </si>
@@ -146,15 +146,6 @@
     <t>O sistema deverá se comunicar com os dados cadastrais de usuários em nosso banco de dados</t>
   </si>
   <si>
-    <t>Usuário clica no botão "Voltar"</t>
-  </si>
-  <si>
-    <t>Sistema deve retornar o Site Institucional da Aplicação do projeto Hunter</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Em situação de erro de preenchimento, o usuário deverá ser avisado e ter a oportunidade de digitar novamente seus dados. Com os dados corretos, após o mesmo ser armazenado em nosso banco de Dados, o usuário deverá ser direcionado a Tela de Dontinuação de Cadastro do projeto Hunter</t>
-  </si>
-  <si>
     <t>Continuação do cadastro do usuário</t>
   </si>
   <si>
@@ -180,6 +171,63 @@
   </si>
   <si>
     <t>Com as escolhas corretas, as mesmas serão armazenadas em nosso banco de dados, atrelado a essa ação, o usuário será direcionado a tela de Home da aplicação do projeto Hunter</t>
+  </si>
+  <si>
+    <t>Configurações</t>
+  </si>
+  <si>
+    <t>Usuário acessa a página de configurações</t>
+  </si>
+  <si>
+    <t>O sistema deve exibir a tela de configurações da aplicação, com os dados do usuario</t>
+  </si>
+  <si>
+    <t>Usuário altera as informações necessarias</t>
+  </si>
+  <si>
+    <t>O sistema deverá alterar os dados em nosso banco</t>
+  </si>
+  <si>
+    <t>Usuário clica no botão Salvar</t>
+  </si>
+  <si>
+    <t>O sistema deverá retornar a tela inicial de nossa aplicação caso as informações estejam corretas</t>
+  </si>
+  <si>
+    <t>Perfil do jogador</t>
+  </si>
+  <si>
+    <t>Usuário acessa a página de Perfil</t>
+  </si>
+  <si>
+    <t>O sistema deve exibir a tela de perfil da aplicação, com a foto e pontuação do jogador e os dados de jogos atuais, ultimas partidas e equipes atuais</t>
+  </si>
+  <si>
+    <t>Perfil da equipe</t>
+  </si>
+  <si>
+    <t>Usuário acessa a página de Perfil da equipe</t>
+  </si>
+  <si>
+    <t>O sistema deve exibir a tela de equipe da aplicação, com a foto e pontuação da equipe e os dados de jogadores, ultimas partidas e jogos atuais</t>
+  </si>
+  <si>
+    <t>Usuário insere login ou senha incorretos</t>
+  </si>
+  <si>
+    <t>O sistema deverá retornar um pop-up apontando que um dos campos estão incorretos e permanecer na tela de login</t>
+  </si>
+  <si>
+    <t>UAT_A_011</t>
+  </si>
+  <si>
+    <t>UAT_A_012</t>
+  </si>
+  <si>
+    <t>Com os dados corretos, após o mesmo ser armazenado em nosso banco de Dados, o usuário deverá ser direcionado a Tela de continuação de Cadastro do projeto Hunter</t>
+  </si>
+  <si>
+    <t>Em situação de erro de preenchimento, o usuário deverá ser avisado e ter a oportunidade de digitar novamente seus dados.</t>
   </si>
 </sst>
 </file>
@@ -240,14 +288,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,7 +614,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +625,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -588,7 +636,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -597,7 +645,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -606,12 +654,12 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -661,11 +709,88 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56CACC0-D405-4DA8-B8A6-077CAD7A68D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D53305D5-B540-4BFE-BA81-2DFA2BF408E0}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAA44DC-3DD9-4458-9AA3-B8D422510AB8}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,21 +799,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>25</v>
+      <c r="A1" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="7"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="7"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56CACC0-D405-4DA8-B8A6-077CAD7A68D7}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -699,11 +862,110 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3D3A43-3A9E-4AA7-8B1E-537360855541}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="267" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80CEFA5-6735-4CD9-AC59-D924DA2618BB}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C5"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,8 +976,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
+      <c r="A1" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -725,7 +987,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -734,7 +996,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -743,12 +1005,12 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -797,7 +1059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEC739F-6ED4-4FBB-9B6D-532D99CDF9EA}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -813,8 +1075,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>18</v>
+      <c r="A1" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -824,7 +1086,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
@@ -833,7 +1095,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -842,12 +1104,12 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -855,14 +1117,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>28</v>
       </c>
     </row>
@@ -870,34 +1132,28 @@
       <c r="A7" s="2">
         <v>2</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>4</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="C8" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -916,12 +1172,116 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37487F9-8D4C-4208-8D67-3826C081A042}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD546F0-FDFF-4749-99C1-D833D04C885B}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,8 +1292,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>19</v>
+      <c r="A1" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -943,7 +1303,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -952,7 +1312,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -961,12 +1321,12 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -974,59 +1334,59 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>40</v>
+      <c r="B7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>42</v>
+      <c r="B8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>44</v>
+      <c r="B9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>45</v>
+      <c r="B10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1046,46 +1406,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E121097-8404-41AE-9FE2-0519B88B3910}">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:A5"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B472FB-5909-4047-9318-E6AD5E5B4018}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1098,59 +1420,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>21</v>
+      <c r="A1" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="7"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="7"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:A5"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F83F4D-E66C-40FF-8308-FE5308B374E1}">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1161,8 +1445,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D53305D5-B540-4BFE-BA81-2DFA2BF408E0}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B472FB-5909-4047-9318-E6AD5E5B4018}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A5"/>
@@ -1170,25 +1454,86 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1199,8 +1544,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAA44DC-3DD9-4458-9AA3-B8D422510AB8}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F83F4D-E66C-40FF-8308-FE5308B374E1}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A5"/>
@@ -1208,25 +1553,64 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Documento de layout e arquivo de esportacao
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de Testes (UAT).xlsx
+++ b/Documentação/Planilha de Testes (UAT).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghgoncalves\Desktop\project-hunter\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08400C63-355A-415A-B493-0161B42421BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4835F61-D436-461F-813C-403C1180D29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="9" activeTab="13" xr2:uid="{CCEB0146-9C4B-423C-9F76-223A38A39EE4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="943" firstSheet="7" activeTab="13" xr2:uid="{CCEB0146-9C4B-423C-9F76-223A38A39EE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="3" r:id="rId1"/>
@@ -27,6 +27,8 @@
     <sheet name="Perfil do Jogador" sheetId="6" r:id="rId12"/>
     <sheet name="Perfil da Equipe" sheetId="7" r:id="rId13"/>
     <sheet name="Buscar" sheetId="9" r:id="rId14"/>
+    <sheet name="Agendar partidas" sheetId="17" r:id="rId15"/>
+    <sheet name="Planilha2" sheetId="18" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="79">
   <si>
     <t>UAT_A_001</t>
   </si>
@@ -199,12 +201,6 @@
     <t>Perfil da equipe</t>
   </si>
   <si>
-    <t>Usuário acessa a página de Perfil da equipe</t>
-  </si>
-  <si>
-    <t>O sistema deve exibir a tela de equipe da aplicação, com a foto e pontuação da equipe e os dados de jogadores, ultimas partidas e jogos atuais</t>
-  </si>
-  <si>
     <t>Usuário insere login ou senha incorretos</t>
   </si>
   <si>
@@ -251,6 +247,42 @@
   </si>
   <si>
     <t>UAT_A_0??</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Usuário conecta a plataforma através de seu login</t>
+  </si>
+  <si>
+    <t>Sistema deve apresentar a tela principal da plataforma; contendo o agendamento de partidas do dia atual; barra de pesquisas na parte superior central da interface; opção de criação de partidas abaixo das partidas já agendas; um botão na parte superior direita da plataforma para acessos as informações pessoais;</t>
+  </si>
+  <si>
+    <t>Agendar partidas</t>
+  </si>
+  <si>
+    <t>Usuário acessa a opção de agendar partidas através da interface principal da plataforma</t>
+  </si>
+  <si>
+    <t>A plataforma deve apresentar uma tela contendo um campo de seleção para adicionar outros jogadores opcionais e suas posições e  opções já pré definidas com os seguintes campos: Selecione um jogo; Selecione sua posição; Selecione um horário; Selecione o dia;</t>
+  </si>
+  <si>
+    <t>Usuário clica em "Criar"</t>
+  </si>
+  <si>
+    <t>Usuário clica em "Fechar"</t>
+  </si>
+  <si>
+    <t>Em ambiente de desistência na criação da partida, a tela principal (Home), deverá ser apresentada ao uuário.</t>
+  </si>
+  <si>
+    <t>Em ambiente de dados selecionados com êxitos, os mesmos devem ser armazenados em nosso banco de dados e ficarem visíveis ao usuário em sua tela de partidas agendadas (Home).</t>
+  </si>
+  <si>
+    <t>O sistema deve exibir a tela de equipe da aplicação, com a foto e pontuação da equipe e os dados de jogadores, ultimas partidas e jogos atuais.</t>
+  </si>
+  <si>
+    <t>Usuário acessa a página de Perfil da equipe.</t>
   </si>
 </sst>
 </file>
@@ -297,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,6 +351,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,10 +840,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.25">
@@ -898,10 +933,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -917,7 +952,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +964,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -994,19 +1029,19 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="58.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1047,15 +1082,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>52</v>
+      <c r="B6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1071,7 +1106,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1116,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1100,6 +1135,108 @@
   <mergeCells count="1">
     <mergeCell ref="A1:A5"/>
   </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB07192-3C84-478A-9C73-4489C5E4EB9B}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="68.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7306ADC7-82CC-4559-AD77-88C51DC3E76E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -1115,8 +1252,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1162,7 +1299,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1173,18 +1310,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="267" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1192,7 +1329,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1208,7 +1345,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,10 +1513,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1483,7 +1620,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1585,7 +1722,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -1596,7 +1733,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -1744,33 +1881,72 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E121097-8404-41AE-9FE2-0519B88B3910}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1785,7 +1961,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B1" sqref="B1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,7 +2030,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Modelando paginas para ficar onePage
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de Testes (UAT).xlsx
+++ b/Documentação/Planilha de Testes (UAT).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghgoncalves\Desktop\project-hunter\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a08d7f3c16d54179/Área de Trabalho/Projeto/project-hunter/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4835F61-D436-461F-813C-403C1180D29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F4835F61-D436-461F-813C-403C1180D29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{98AD022D-F7FA-40B7-969D-E29260308B4C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="943" firstSheet="7" activeTab="13" xr2:uid="{CCEB0146-9C4B-423C-9F76-223A38A39EE4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="943" firstSheet="5" activeTab="14" xr2:uid="{CCEB0146-9C4B-423C-9F76-223A38A39EE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <sheet name="Perfil da Equipe" sheetId="7" r:id="rId13"/>
     <sheet name="Buscar" sheetId="9" r:id="rId14"/>
     <sheet name="Agendar partidas" sheetId="17" r:id="rId15"/>
-    <sheet name="Planilha2" sheetId="18" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -349,11 +348,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,18 +671,18 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="A1:C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -693,8 +692,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -702,8 +701,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -711,13 +710,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -725,7 +724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -736,7 +735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -747,7 +746,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -774,15 +773,15 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -792,8 +791,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -801,8 +800,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -810,13 +809,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -824,7 +823,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -835,7 +834,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -846,7 +845,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -867,15 +866,15 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -885,8 +884,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -894,8 +893,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -903,13 +902,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -917,7 +916,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -928,7 +927,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -955,15 +954,15 @@
       <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -973,8 +972,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -982,8 +981,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -991,13 +990,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1005,7 +1004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="127.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1032,15 +1031,15 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="58.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
+    <col min="3" max="3" width="58.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1050,8 +1049,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1059,8 +1058,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1068,13 +1067,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1082,7 +1081,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1105,31 +1104,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAA44DC-3DD9-4458-9AA3-B8D422510AB8}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1143,19 +1142,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB07192-3C84-478A-9C73-4489C5E4EB9B}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="68.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.88671875" customWidth="1"/>
+    <col min="3" max="3" width="68.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1165,8 +1164,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1174,8 +1173,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1183,21 +1182,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>71</v>
       </c>
@@ -1205,7 +1204,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>73</v>
       </c>
@@ -1213,7 +1212,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>74</v>
       </c>
@@ -1225,18 +1224,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:A5"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7306ADC7-82CC-4559-AD77-88C51DC3E76E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -1249,15 +1236,15 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="54.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
+    <col min="3" max="3" width="54.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1267,8 +1254,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1276,8 +1263,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1285,13 +1272,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1299,7 +1286,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1310,7 +1297,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1321,7 +1308,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1348,15 +1335,15 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" customWidth="1"/>
+    <col min="3" max="3" width="50.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1366,8 +1353,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1375,8 +1362,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1384,13 +1371,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1398,7 +1385,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1409,7 +1396,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1420,7 +1407,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1447,15 +1434,15 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1465,8 +1452,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1474,8 +1461,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1483,13 +1470,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1497,7 +1484,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1508,7 +1495,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1519,7 +1506,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="184.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1540,15 +1527,15 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1558,8 +1545,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1567,8 +1554,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1576,13 +1563,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1590,7 +1577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1601,7 +1588,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1612,7 +1599,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1623,18 +1610,18 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
     </row>
   </sheetData>
@@ -1653,15 +1640,15 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1671,8 +1658,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1680,8 +1667,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1689,13 +1676,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1703,7 +1690,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1714,7 +1701,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1725,7 +1712,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1736,7 +1723,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5"/>
@@ -1757,15 +1744,15 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" customWidth="1"/>
     <col min="3" max="3" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1775,8 +1762,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1784,8 +1771,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1793,13 +1780,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1807,7 +1794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1818,7 +1805,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1829,7 +1816,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1840,7 +1827,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -1851,7 +1838,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>5</v>
       </c>
@@ -1862,13 +1849,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
     </row>
   </sheetData>
@@ -1887,15 +1874,15 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.44140625" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1905,8 +1892,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1914,8 +1901,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1923,13 +1910,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1937,7 +1924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1964,15 +1951,15 @@
       <selection activeCell="B1" sqref="B1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1982,8 +1969,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1991,8 +1978,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2000,13 +1987,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2014,7 +2001,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -2025,7 +2012,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -2036,7 +2023,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>

</xml_diff>

<commit_message>
Enter nos botões (Realizado pelo Henrique)
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de Testes (UAT).xlsx
+++ b/Documentação/Planilha de Testes (UAT).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghgoncalves\Desktop\project-hunter\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA28B71-634F-4FC5-B36E-460564FABD60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2526BAD1-C232-4BB4-B85A-32D1FE820030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="943" xr2:uid="{CCEB0146-9C4B-423C-9F76-223A38A39EE4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="943" activeTab="7" xr2:uid="{CCEB0146-9C4B-423C-9F76-223A38A39EE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="3" r:id="rId1"/>
@@ -167,9 +167,6 @@
     <t>Usuário clica em continuar</t>
   </si>
   <si>
-    <t xml:space="preserve">Ambiente de Jogo e Posição não escolhida, um alerta será enviado ao usuário e o mesmo terá a oporunidade de seleção de novamente. </t>
-  </si>
-  <si>
     <t>Com as escolhas corretas, as mesmas serão armazenadas em nosso banco de dados, atrelado a essa ação, o usuário será direcionado a tela de Home da aplicação do projeto Hunter</t>
   </si>
   <si>
@@ -297,6 +294,9 @@
   </si>
   <si>
     <t>UAT_A_015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambiente de Jogo e/ou Posição não escolhida, um alerta será enviado ao usuário e o mesmo terá a oporunidade de seleção de novamente. </t>
   </si>
 </sst>
 </file>
@@ -548,20 +548,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -585,6 +576,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1641,7 +1641,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1990725" cy="2286000"/>
+          <a:ext cx="1990725" cy="2095500"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="1990725" cy="2466976"/>
         </a:xfrm>
@@ -2271,7 +2271,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1990725" cy="2657474"/>
+          <a:ext cx="1990725" cy="2466974"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="1990725" cy="2466976"/>
         </a:xfrm>
@@ -2793,7 +2793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF6AEAB-FBF6-43E5-8942-7553830315CA}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2807,7 +2807,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
@@ -2818,8 +2818,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -2828,66 +2828,66 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="16" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="16" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2933,19 +2933,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -2954,55 +2954,55 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>43</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>44</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>45</v>
+        <v>57</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>44</v>
       </c>
       <c r="E7" s="7"/>
     </row>
@@ -3048,19 +3048,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
-        <v>51</v>
+      <c r="B1" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -3069,55 +3069,55 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>43</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>44</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>60</v>
       </c>
       <c r="E7" s="7"/>
     </row>
@@ -3163,19 +3163,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
-        <v>52</v>
+      <c r="B1" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -3184,55 +3184,55 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>43</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>44</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>61</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>62</v>
       </c>
       <c r="E7" s="7"/>
     </row>
@@ -3278,19 +3278,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
-        <v>81</v>
+      <c r="B1" s="21" t="s">
+        <v>80</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -3299,42 +3299,42 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>80</v>
+        <v>46</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="E6" s="7"/>
     </row>
@@ -3380,19 +3380,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
-        <v>82</v>
+      <c r="B1" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -3401,54 +3401,54 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>77</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3488,19 +3488,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
-        <v>83</v>
+      <c r="B1" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -3509,67 +3509,67 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>68</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="14">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
-        <v>3</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3614,7 +3614,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
@@ -3625,8 +3625,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -3635,67 +3635,67 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>50</v>
+      <c r="D8" s="16" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3740,7 +3740,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="8" t="s">
@@ -3751,8 +3751,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -3761,66 +3761,66 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="16" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3866,7 +3866,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="8" t="s">
@@ -3877,8 +3877,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -3887,62 +3887,62 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="18"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>55</v>
-      </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="19"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
@@ -3986,7 +3986,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="8" t="s">
@@ -3997,8 +3997,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -4007,67 +4007,67 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="18"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="16" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>56</v>
+      <c r="D8" s="16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -4112,7 +4112,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="24" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="8" t="s">
@@ -4123,8 +4123,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -4133,67 +4133,67 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="18"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>57</v>
+      <c r="D7" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>53</v>
+      <c r="D8" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -4238,20 +4238,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="25"/>
+      <c r="C2" s="20" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="23" t="s">
-        <v>75</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>6</v>
@@ -4259,78 +4259,78 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="18"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="16" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="7"/>
     </row>
@@ -4362,8 +4362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAA44DC-3DD9-4458-9AA3-B8D422510AB8}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4376,19 +4376,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -4397,78 +4397,78 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="16" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="E9" s="7"/>
     </row>
@@ -4514,19 +4514,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -4535,42 +4535,42 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="12"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>64</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>65</v>
       </c>
       <c r="E6" s="7"/>
     </row>

</xml_diff>